<commit_message>
Lösung Übung 2 und 3
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Netzplan_Übung.xlsx
+++ b/FIAEB Übungen/Netzplan_Übung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FIAEB Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D2BD8B-C223-40F2-BB06-09FA59827821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4FD4AD-C42E-446D-82E8-7022EA1429F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übung1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>kritischer Pfad</t>
+  </si>
+  <si>
+    <t>FP = kleinste FAZ(Nachfolger)- FEZ</t>
   </si>
 </sst>
 </file>
@@ -666,7 +669,79 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="51">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2513,67 +2588,67 @@
     <mergeCell ref="H39:P39"/>
   </mergeCells>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="42" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="39" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27">
-    <cfRule type="cellIs" dxfId="33" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V17">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA17">
-    <cfRule type="cellIs" dxfId="30" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2590,8 +2665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -2786,21 +2861,50 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="15"/>
+      <c r="A12" s="15">
+        <v>0</v>
+      </c>
       <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="F12" s="15"/>
+      <c r="C12" s="17">
+        <f>A12+A14</f>
+        <v>6</v>
+      </c>
+      <c r="F12" s="15">
+        <f>C12</f>
+        <v>6</v>
+      </c>
       <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
-      <c r="K12" s="15"/>
+      <c r="H12" s="17">
+        <f>F12+F14</f>
+        <v>13</v>
+      </c>
+      <c r="K12" s="15">
+        <f>H12</f>
+        <v>13</v>
+      </c>
       <c r="L12" s="16"/>
-      <c r="M12" s="17"/>
-      <c r="P12" s="15"/>
+      <c r="M12" s="17">
+        <f>K12+K14</f>
+        <v>17</v>
+      </c>
+      <c r="P12" s="15">
+        <f>M12</f>
+        <v>17</v>
+      </c>
       <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
-      <c r="U12" s="15"/>
+      <c r="R12" s="17">
+        <f>P12+P14</f>
+        <v>20</v>
+      </c>
+      <c r="U12" s="15">
+        <f>MAX(R12,R18)</f>
+        <v>24</v>
+      </c>
       <c r="V12" s="16"/>
-      <c r="W12" s="17"/>
+      <c r="W12" s="17">
+        <f>U12+U14</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="13.5" thickBot="1">
       <c r="A13" s="42" t="s">
@@ -2842,54 +2946,113 @@
         <f>VLOOKUP(A13,$A$2:$H$10,8)</f>
         <v>6</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="19">
+        <f>C15-C12</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="20">
+        <f>MIN(F12,F18)-C12</f>
+        <v>0</v>
+      </c>
       <c r="D14" s="25"/>
       <c r="F14" s="18">
         <f>VLOOKUP(F13,$A$2:$H$10,8)</f>
         <v>7</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
+      <c r="G14" s="19">
+        <f>H15-H12</f>
+        <v>4</v>
+      </c>
+      <c r="H14" s="20">
+        <f>K12-H12</f>
+        <v>0</v>
+      </c>
       <c r="K14" s="18">
         <f>VLOOKUP(K13,$A$2:$H$10,8)</f>
         <v>4</v>
       </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="20"/>
+      <c r="L14" s="19">
+        <f>M15-M12</f>
+        <v>4</v>
+      </c>
+      <c r="M14" s="20">
+        <f>P12-M12</f>
+        <v>0</v>
+      </c>
       <c r="P14" s="18">
         <f>VLOOKUP(P13,$A$2:$H$10,8)</f>
         <v>3</v>
       </c>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="20"/>
+      <c r="Q14" s="19">
+        <f>R15-R12</f>
+        <v>4</v>
+      </c>
+      <c r="R14" s="20">
+        <f>U12-R12</f>
+        <v>4</v>
+      </c>
       <c r="S14" s="33"/>
       <c r="T14" s="30"/>
       <c r="U14" s="18">
         <f>VLOOKUP(U13,$A$2:$H$10,8)</f>
         <v>2</v>
       </c>
-      <c r="V14" s="19"/>
-      <c r="W14" s="20"/>
+      <c r="V14" s="19">
+        <f>W15-W12</f>
+        <v>0</v>
+      </c>
+      <c r="W14" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="21"/>
+      <c r="A15" s="21">
+        <f>C15-A14</f>
+        <v>0</v>
+      </c>
       <c r="B15" s="16"/>
-      <c r="C15" s="22"/>
+      <c r="C15" s="22">
+        <f>MIN(F15,F21)</f>
+        <v>6</v>
+      </c>
       <c r="D15" s="26"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21">
+        <f>H15-F14</f>
+        <v>10</v>
+      </c>
       <c r="G15" s="16"/>
-      <c r="H15" s="22"/>
-      <c r="K15" s="21"/>
+      <c r="H15" s="22">
+        <f>K15</f>
+        <v>17</v>
+      </c>
+      <c r="K15" s="21">
+        <f>M15-K14</f>
+        <v>17</v>
+      </c>
       <c r="L15" s="16"/>
-      <c r="M15" s="22"/>
-      <c r="P15" s="21"/>
+      <c r="M15" s="22">
+        <f>P15</f>
+        <v>21</v>
+      </c>
+      <c r="P15" s="21">
+        <f>R15-P14</f>
+        <v>21</v>
+      </c>
       <c r="Q15" s="16"/>
-      <c r="R15" s="22"/>
+      <c r="R15" s="22">
+        <f>U15</f>
+        <v>24</v>
+      </c>
       <c r="S15" s="27"/>
-      <c r="U15" s="21"/>
+      <c r="U15" s="21">
+        <f>W15-U14</f>
+        <v>24</v>
+      </c>
       <c r="V15" s="16"/>
-      <c r="W15" s="22"/>
+      <c r="W15" s="22">
+        <f>W12</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="D16" s="27"/>
@@ -2901,15 +3064,33 @@
     </row>
     <row r="18" spans="4:19">
       <c r="D18" s="27"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="15">
+        <f>C12</f>
+        <v>6</v>
+      </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="K18" s="15"/>
+      <c r="H18" s="17">
+        <f>F18+F20</f>
+        <v>13</v>
+      </c>
+      <c r="K18" s="15">
+        <f>H18</f>
+        <v>13</v>
+      </c>
       <c r="L18" s="16"/>
-      <c r="M18" s="17"/>
-      <c r="P18" s="15"/>
+      <c r="M18" s="17">
+        <f>K18+K20</f>
+        <v>17</v>
+      </c>
+      <c r="P18" s="15">
+        <f>MAX(M18,M24)</f>
+        <v>18</v>
+      </c>
       <c r="Q18" s="16"/>
-      <c r="R18" s="17"/>
+      <c r="R18" s="17">
+        <f>P18+P20</f>
+        <v>24</v>
+      </c>
       <c r="S18" s="27"/>
     </row>
     <row r="19" spans="4:19" ht="13.5" thickBot="1">
@@ -2941,35 +3122,71 @@
         <f>VLOOKUP(F19,$A$2:$H$10,8)</f>
         <v>7</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="19">
+        <f>H21-H18</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
+        <f>MIN(K18,K24)-H18</f>
+        <v>0</v>
+      </c>
       <c r="I20" s="25"/>
       <c r="K20" s="18">
         <f>VLOOKUP(K19,$A$2:$H$10,8)</f>
         <v>4</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
+      <c r="L20" s="19">
+        <f>M21-M18</f>
+        <v>1</v>
+      </c>
+      <c r="M20" s="20">
+        <f>P18-M18</f>
+        <v>1</v>
+      </c>
       <c r="O20" s="30"/>
       <c r="P20" s="18">
         <f>VLOOKUP(P19,$A$2:$H$10,8)</f>
         <v>6</v>
       </c>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="20"/>
+      <c r="Q20" s="19">
+        <f>R21-R18</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="20">
+        <f>U12-R18</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="4:19">
-      <c r="F21" s="21"/>
+      <c r="F21" s="21">
+        <f>H21-F20</f>
+        <v>6</v>
+      </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="22"/>
+      <c r="H21" s="22">
+        <f>MIN(K21,K27)</f>
+        <v>13</v>
+      </c>
       <c r="I21" s="26"/>
-      <c r="K21" s="21"/>
+      <c r="K21" s="21">
+        <f>M21-K20</f>
+        <v>14</v>
+      </c>
       <c r="L21" s="16"/>
-      <c r="M21" s="22"/>
+      <c r="M21" s="22">
+        <f>P21</f>
+        <v>18</v>
+      </c>
       <c r="N21" s="27"/>
-      <c r="P21" s="21"/>
+      <c r="P21" s="21">
+        <f>R21-P20</f>
+        <v>18</v>
+      </c>
       <c r="Q21" s="16"/>
-      <c r="R21" s="22"/>
+      <c r="R21" s="22">
+        <f>U15</f>
+        <v>24</v>
+      </c>
     </row>
     <row r="22" spans="4:19">
       <c r="I22" s="27"/>
@@ -2983,12 +3200,12 @@
       <c r="I24" s="27"/>
       <c r="K24" s="15">
         <f>H18</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L24" s="16"/>
       <c r="M24" s="17">
         <f>K24+K26</f>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="N24" s="27"/>
     </row>
@@ -3007,13 +3224,25 @@
         <f>VLOOKUP(K25,$A$2:$H$10,8)</f>
         <v>5</v>
       </c>
-      <c r="L26" s="19"/>
-      <c r="M26" s="20"/>
+      <c r="L26" s="19">
+        <f>M27-M24</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="20">
+        <f>P18-M24</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="4:19">
-      <c r="K27" s="21"/>
+      <c r="K27" s="21">
+        <f>M27-K26</f>
+        <v>13</v>
+      </c>
       <c r="L27" s="16"/>
-      <c r="M27" s="22"/>
+      <c r="M27" s="22">
+        <f>P21</f>
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3029,53 +3258,53 @@
     <mergeCell ref="K19:M19"/>
     <mergeCell ref="P19:R19"/>
   </mergeCells>
-  <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V14">
+    <cfRule type="cellIs" dxfId="28" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q14">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q20">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="20" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3093,7 +3322,7 @@
   <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -3270,6 +3499,16 @@
       <c r="H9" s="3">
         <v>15</v>
       </c>
+      <c r="P9" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" s="3" t="s">
@@ -3290,18 +3529,34 @@
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="15"/>
+      <c r="A12" s="15">
+        <v>0</v>
+      </c>
       <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="F12" s="15"/>
+      <c r="C12" s="17">
+        <v>15</v>
+      </c>
+      <c r="F12" s="15">
+        <v>15</v>
+      </c>
       <c r="G12" s="16"/>
-      <c r="H12" s="17"/>
-      <c r="P12" s="15"/>
+      <c r="H12" s="17">
+        <v>21</v>
+      </c>
+      <c r="P12" s="15">
+        <v>21</v>
+      </c>
       <c r="Q12" s="16"/>
-      <c r="R12" s="17"/>
-      <c r="U12" s="15"/>
+      <c r="R12" s="17">
+        <v>28</v>
+      </c>
+      <c r="U12" s="15">
+        <v>59</v>
+      </c>
       <c r="V12" s="16"/>
-      <c r="W12" s="17"/>
+      <c r="W12" s="17">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:23" ht="13.5" thickBot="1">
       <c r="A13" s="42" t="s">
@@ -3341,45 +3596,77 @@
         <f>VLOOKUP(A13,$A$2:$H$10,8)</f>
         <v>15</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="19">
+        <v>0</v>
+      </c>
+      <c r="C14" s="20">
+        <v>0</v>
+      </c>
       <c r="D14" s="25"/>
       <c r="F14" s="18">
         <f>VLOOKUP(F13,$A$2:$H$10,8)</f>
         <v>6</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="20"/>
+      <c r="G14" s="19">
+        <v>31</v>
+      </c>
+      <c r="H14" s="20">
+        <v>0</v>
+      </c>
       <c r="P14" s="18">
         <f>VLOOKUP(P13,$A$2:$H$10,8)</f>
         <v>7</v>
       </c>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="20"/>
+      <c r="Q14" s="19">
+        <v>31</v>
+      </c>
+      <c r="R14" s="20">
+        <v>31</v>
+      </c>
       <c r="S14" s="33"/>
       <c r="T14" s="30"/>
       <c r="U14" s="18">
         <f>VLOOKUP(U13,$A$2:$H$10,8)</f>
         <v>4</v>
       </c>
-      <c r="V14" s="19"/>
-      <c r="W14" s="20"/>
+      <c r="V14" s="19">
+        <v>0</v>
+      </c>
+      <c r="W14" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="21"/>
+      <c r="A15" s="21">
+        <v>0</v>
+      </c>
       <c r="B15" s="16"/>
-      <c r="C15" s="22"/>
+      <c r="C15" s="22">
+        <v>15</v>
+      </c>
       <c r="D15" s="26"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21">
+        <v>46</v>
+      </c>
       <c r="G15" s="16"/>
-      <c r="H15" s="22"/>
-      <c r="P15" s="21"/>
+      <c r="H15" s="22">
+        <v>52</v>
+      </c>
+      <c r="P15" s="21">
+        <v>52</v>
+      </c>
       <c r="Q15" s="16"/>
-      <c r="R15" s="22"/>
+      <c r="R15" s="22">
+        <v>59</v>
+      </c>
       <c r="S15" s="27"/>
-      <c r="U15" s="21"/>
+      <c r="U15" s="21">
+        <v>59</v>
+      </c>
       <c r="V15" s="16"/>
-      <c r="W15" s="22"/>
+      <c r="W15" s="22">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:23">
       <c r="C16" s="38"/>
@@ -3394,15 +3681,27 @@
     <row r="18" spans="3:19">
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="F18" s="15"/>
+      <c r="F18" s="15">
+        <v>15</v>
+      </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="17"/>
-      <c r="K18" s="15"/>
+      <c r="H18" s="17">
+        <v>29</v>
+      </c>
+      <c r="K18" s="15">
+        <v>29</v>
+      </c>
       <c r="L18" s="16"/>
-      <c r="M18" s="17"/>
-      <c r="P18" s="15"/>
+      <c r="M18" s="17">
+        <v>44</v>
+      </c>
+      <c r="P18" s="15">
+        <v>44</v>
+      </c>
       <c r="Q18" s="16"/>
-      <c r="R18" s="17"/>
+      <c r="R18" s="17">
+        <v>59</v>
+      </c>
       <c r="S18" s="27"/>
     </row>
     <row r="19" spans="3:19" ht="13.5" thickBot="1">
@@ -3436,35 +3735,59 @@
         <f>VLOOKUP(F19,$A$2:$H$10,8)</f>
         <v>14</v>
       </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="20"/>
+      <c r="G20" s="19">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
+        <v>0</v>
+      </c>
       <c r="I20" s="33"/>
       <c r="K20" s="18">
         <f>VLOOKUP(K19,$A$2:$H$10,8)</f>
         <v>15</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
+      <c r="L20" s="19">
+        <v>0</v>
+      </c>
+      <c r="M20" s="20">
+        <v>0</v>
+      </c>
       <c r="O20" s="30"/>
       <c r="P20" s="18">
         <f>VLOOKUP(P19,$A$2:$H$10,8)</f>
         <v>15</v>
       </c>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="20"/>
+      <c r="Q20" s="19">
+        <v>0</v>
+      </c>
+      <c r="R20" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="3:19">
       <c r="C21" s="27"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="21">
+        <v>15</v>
+      </c>
       <c r="G21" s="16"/>
-      <c r="H21" s="34"/>
-      <c r="K21" s="36"/>
+      <c r="H21" s="34">
+        <v>29</v>
+      </c>
+      <c r="K21" s="36">
+        <v>29</v>
+      </c>
       <c r="L21" s="16"/>
-      <c r="M21" s="22"/>
+      <c r="M21" s="22">
+        <v>44</v>
+      </c>
       <c r="N21" s="27"/>
-      <c r="P21" s="36"/>
+      <c r="P21" s="36">
+        <v>44</v>
+      </c>
       <c r="Q21" s="16"/>
-      <c r="R21" s="22"/>
+      <c r="R21" s="22">
+        <v>59</v>
+      </c>
     </row>
     <row r="22" spans="3:19">
       <c r="C22" s="27"/>
@@ -3476,17 +3799,19 @@
     </row>
     <row r="24" spans="3:19">
       <c r="C24" s="27"/>
-      <c r="F24" s="15"/>
+      <c r="F24" s="15">
+        <v>15</v>
+      </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="35">
+        <v>21</v>
+      </c>
       <c r="K24" s="37">
-        <f>H18</f>
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L24" s="16"/>
       <c r="M24" s="17">
-        <f>K24+K26</f>
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="N24" s="27"/>
     </row>
@@ -3513,25 +3838,42 @@
         <f>VLOOKUP(F25,$A$2:$H$10,8)</f>
         <v>6</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="20"/>
+      <c r="G26" s="19">
+        <v>9</v>
+      </c>
+      <c r="H26" s="20">
+        <v>0</v>
+      </c>
       <c r="K26" s="18">
         <f>VLOOKUP(K25,$A$2:$H$10,8)</f>
         <v>14</v>
       </c>
-      <c r="L26" s="19"/>
-      <c r="M26" s="20"/>
+      <c r="L26" s="19">
+        <v>9</v>
+      </c>
+      <c r="M26" s="20">
+        <v>9</v>
+      </c>
     </row>
     <row r="27" spans="3:19">
-      <c r="F27" s="21"/>
+      <c r="F27" s="21">
+        <v>24</v>
+      </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="22"/>
-      <c r="K27" s="21"/>
+      <c r="H27" s="22">
+        <v>30</v>
+      </c>
+      <c r="K27" s="21">
+        <v>30</v>
+      </c>
       <c r="L27" s="16"/>
-      <c r="M27" s="22"/>
+      <c r="M27" s="22">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="P9:W9"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A13:C13"/>
@@ -3545,47 +3887,47 @@
     <mergeCell ref="P13:R13"/>
   </mergeCells>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="19" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3602,7 +3944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{559B4883-E629-4891-9D84-A4D18D9F93F4}">
   <dimension ref="A1:AB29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -4141,57 +4483,57 @@
     <mergeCell ref="U15:W15"/>
   </mergeCells>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA19">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Netzplan (Aufwandsplanung) mit allen Formeln (/\)
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Netzplan_Übung.xlsx
+++ b/FIAEB Übungen/Netzplan_Übung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FIAEB Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66501CF3-8106-40CC-8160-207459A1E3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D085A4-3695-431A-873B-DF80DF2C26CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -688,7 +688,97 @@
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="73">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1644,14 +1734,14 @@
   <dimension ref="A1:AD67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="Z17" sqref="Z17"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -1700,14 +1790,14 @@
         <v>2</v>
       </c>
       <c r="I2" s="48">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J2" s="49">
         <v>1</v>
       </c>
       <c r="K2" s="3">
         <f>ROUNDUP(H2/(I2*J2),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" s="6"/>
     </row>
@@ -2044,42 +2134,53 @@
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="17">
-        <v>2</v>
+        <f>A15+A17</f>
+        <v>1</v>
       </c>
       <c r="F15" s="15">
-        <v>2</v>
+        <f>C15</f>
+        <v>1</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="17">
-        <v>10</v>
+        <f>F15+F17</f>
+        <v>5</v>
       </c>
       <c r="K15" s="15">
-        <v>10</v>
+        <f>H15</f>
+        <v>5</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15" s="17">
-        <v>16</v>
+        <f>K15+K17</f>
+        <v>11</v>
       </c>
       <c r="P15" s="15">
-        <v>16</v>
+        <f>M15</f>
+        <v>11</v>
       </c>
       <c r="Q15" s="16"/>
       <c r="R15" s="17">
-        <v>21</v>
+        <f>P15+P17</f>
+        <v>16</v>
       </c>
       <c r="U15" s="15">
-        <v>21</v>
+        <f>R15</f>
+        <v>16</v>
       </c>
       <c r="V15" s="16"/>
       <c r="W15" s="17">
-        <v>29</v>
+        <f>U15+U17</f>
+        <v>24</v>
       </c>
       <c r="Z15" s="15">
-        <v>29</v>
+        <f>MAX(W15,W20)</f>
+        <v>25</v>
       </c>
       <c r="AA15" s="16"/>
       <c r="AB15" s="17">
-        <v>33</v>
+        <f>Z15+Z17</f>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="13.5" thickBot="1">
@@ -2127,9 +2228,10 @@
     <row r="17" spans="1:30" ht="13.5" thickBot="1">
       <c r="A17" s="18">
         <f>VLOOKUP(A16,$A$2:$K$13,11)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="19">
+        <f>C18-C15</f>
         <v>0</v>
       </c>
       <c r="C17" s="20"/>
@@ -2139,7 +2241,8 @@
         <v>4</v>
       </c>
       <c r="G17" s="19">
-        <v>0</v>
+        <f>H18-H15</f>
+        <v>5</v>
       </c>
       <c r="H17" s="20"/>
       <c r="K17" s="18">
@@ -2147,7 +2250,8 @@
         <v>6</v>
       </c>
       <c r="L17" s="19">
-        <v>0</v>
+        <f>M18-M15</f>
+        <v>5</v>
       </c>
       <c r="M17" s="20"/>
       <c r="P17" s="18">
@@ -2155,7 +2259,8 @@
         <v>5</v>
       </c>
       <c r="Q17" s="19">
-        <v>0</v>
+        <f>R18-R15</f>
+        <v>1</v>
       </c>
       <c r="R17" s="20"/>
       <c r="U17" s="18">
@@ -2163,7 +2268,8 @@
         <v>8</v>
       </c>
       <c r="V17" s="19">
-        <v>0</v>
+        <f>W18-W15</f>
+        <v>1</v>
       </c>
       <c r="W17" s="20"/>
       <c r="Y17" s="30"/>
@@ -2172,6 +2278,7 @@
         <v>4</v>
       </c>
       <c r="AA17" s="19">
+        <f>AB18-AB15</f>
         <v>0</v>
       </c>
       <c r="AB17" s="20"/>
@@ -2181,25 +2288,31 @@
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="21">
+        <f>C18-A17</f>
         <v>0</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="22">
-        <v>2</v>
+        <f>MIN(F18,F23)</f>
+        <v>1</v>
       </c>
       <c r="D18" s="26"/>
       <c r="F18" s="21">
-        <v>2</v>
+        <f>H18-F17</f>
+        <v>6</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="22">
+        <f>K18</f>
         <v>10</v>
       </c>
       <c r="K18" s="21">
+        <f>M18-K17</f>
         <v>10</v>
       </c>
       <c r="L18" s="16"/>
       <c r="M18" s="22">
+        <f>P18</f>
         <v>16</v>
       </c>
       <c r="P18" s="21">
@@ -2207,22 +2320,27 @@
       </c>
       <c r="Q18" s="16"/>
       <c r="R18" s="22">
-        <v>21</v>
+        <f>U18</f>
+        <v>17</v>
       </c>
       <c r="U18" s="21">
-        <v>21</v>
+        <f>W18-U17</f>
+        <v>17</v>
       </c>
       <c r="V18" s="16"/>
       <c r="W18" s="22">
-        <v>29</v>
+        <f>Z18</f>
+        <v>25</v>
       </c>
       <c r="X18" s="27"/>
       <c r="Z18" s="21">
-        <v>29</v>
+        <f>AB18-Z17</f>
+        <v>25</v>
       </c>
       <c r="AA18" s="16"/>
       <c r="AB18" s="22">
-        <v>33</v>
+        <f>AB15</f>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -2232,32 +2350,40 @@
     <row r="20" spans="1:30">
       <c r="D20" s="27"/>
       <c r="F20" s="15">
-        <v>2</v>
+        <f>C15</f>
+        <v>1</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="17">
-        <v>10</v>
+        <f>F20+F22</f>
+        <v>9</v>
       </c>
       <c r="K20" s="15">
-        <v>10</v>
+        <f>H20</f>
+        <v>9</v>
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="17">
-        <v>18</v>
+        <f>K20+K22</f>
+        <v>17</v>
       </c>
       <c r="P20" s="15">
-        <v>18</v>
+        <f>M20</f>
+        <v>17</v>
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="17">
-        <v>24</v>
+        <f>P20+P22</f>
+        <v>23</v>
       </c>
       <c r="U20" s="15">
-        <v>24</v>
+        <f>MAX(R20,R25)</f>
+        <v>23</v>
       </c>
       <c r="V20" s="16"/>
       <c r="W20" s="17">
-        <v>26</v>
+        <f>U20+U22</f>
+        <v>25</v>
       </c>
       <c r="X20" s="27"/>
     </row>
@@ -2298,7 +2424,8 @@
         <v>8</v>
       </c>
       <c r="G22" s="19">
-        <v>3</v>
+        <f>H23-H20</f>
+        <v>0</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="25"/>
@@ -2307,7 +2434,8 @@
         <v>8</v>
       </c>
       <c r="L22" s="19">
-        <v>3</v>
+        <f>M23-M20</f>
+        <v>0</v>
       </c>
       <c r="M22" s="20"/>
       <c r="P22" s="18">
@@ -2315,7 +2443,8 @@
         <v>6</v>
       </c>
       <c r="Q22" s="19">
-        <v>3</v>
+        <f>R23-R20</f>
+        <v>0</v>
       </c>
       <c r="R22" s="20"/>
       <c r="T22" s="24"/>
@@ -2324,40 +2453,49 @@
         <v>2</v>
       </c>
       <c r="V22" s="19">
-        <v>3</v>
+        <f>W23-W20</f>
+        <v>0</v>
       </c>
       <c r="W22" s="20"/>
     </row>
     <row r="23" spans="1:30">
       <c r="F23" s="21">
-        <v>5</v>
+        <f>H23-F22</f>
+        <v>1</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="22">
-        <v>13</v>
+        <f>MIN(K23,K28)</f>
+        <v>9</v>
       </c>
       <c r="I23" s="26"/>
       <c r="K23" s="21">
-        <v>13</v>
+        <f>M23-K22</f>
+        <v>9</v>
       </c>
       <c r="L23" s="16"/>
       <c r="M23" s="22">
-        <v>21</v>
+        <f>P23</f>
+        <v>17</v>
       </c>
       <c r="P23" s="21">
-        <v>21</v>
+        <f>R23-P22</f>
+        <v>17</v>
       </c>
       <c r="Q23" s="16"/>
       <c r="R23" s="22">
-        <v>27</v>
+        <f>U23</f>
+        <v>23</v>
       </c>
       <c r="S23" s="27"/>
       <c r="U23" s="21">
-        <v>27</v>
+        <f>W23-U22</f>
+        <v>23</v>
       </c>
       <c r="V23" s="16"/>
       <c r="W23" s="22">
-        <v>29</v>
+        <f>Z18</f>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -2367,18 +2505,22 @@
     <row r="25" spans="1:30">
       <c r="I25" s="27"/>
       <c r="K25" s="15">
-        <v>10</v>
+        <f>H20</f>
+        <v>9</v>
       </c>
       <c r="L25" s="16"/>
       <c r="M25" s="17">
-        <v>18</v>
+        <f>K25+K27</f>
+        <v>17</v>
       </c>
       <c r="P25" s="15">
-        <v>18</v>
+        <f>M25</f>
+        <v>17</v>
       </c>
       <c r="Q25" s="16"/>
       <c r="R25" s="17">
-        <v>23</v>
+        <f>P25+P27</f>
+        <v>22</v>
       </c>
       <c r="S25" s="27"/>
     </row>
@@ -2413,24 +2555,29 @@
         <v>5</v>
       </c>
       <c r="Q27" s="19">
-        <v>4</v>
+        <f>R28-R25</f>
+        <v>1</v>
       </c>
       <c r="R27" s="20"/>
     </row>
     <row r="28" spans="1:30">
       <c r="K28" s="21">
-        <v>14</v>
+        <f>M28-K27</f>
+        <v>10</v>
       </c>
       <c r="L28" s="16"/>
       <c r="M28" s="22">
-        <v>22</v>
+        <f>P28</f>
+        <v>18</v>
       </c>
       <c r="P28" s="21">
-        <v>22</v>
+        <f>R28-P27</f>
+        <v>18</v>
       </c>
       <c r="Q28" s="16"/>
       <c r="R28" s="22">
-        <v>27</v>
+        <f>U23</f>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="56.25">
@@ -2808,67 +2955,62 @@
     <mergeCell ref="K16:M16"/>
   </mergeCells>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="62" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="61" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="22" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L27">
+    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17">
-    <cfRule type="cellIs" dxfId="60" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="59" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" dxfId="58" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="57" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="56" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="54" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q27">
-    <cfRule type="cellIs" dxfId="53" priority="4" operator="equal">
+  <conditionalFormatting sqref="Q17 Q27">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V17">
-    <cfRule type="cellIs" dxfId="52" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA17">
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3427,52 +3569,52 @@
     <mergeCell ref="K13:M13"/>
   </mergeCells>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="48" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="44" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="43" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4131,52 +4273,52 @@
     <mergeCell ref="F13:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="39" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="30" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="29" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="27" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4914,57 +5056,57 @@
     <mergeCell ref="U21:W21"/>
   </mergeCells>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA19">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Echt wirklich aller aller letzte Korrektur.
</commit_message>
<xml_diff>
--- a/FIAEB Übungen/Netzplan_Übung.xlsx
+++ b/FIAEB Übungen/Netzplan_Übung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FIAEB Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D085A4-3695-431A-873B-DF80DF2C26CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C59419-EB05-4979-8846-686FAB86046D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -656,11 +656,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -671,276 +683,12 @@
     <xf numFmtId="49" fontId="7" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="73">
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
-    </dxf>
+  <dxfs count="44">
     <dxf>
       <font>
         <b/>
@@ -1208,15 +956,6 @@
           <bgColor rgb="FFCC0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -1734,7 +1473,7 @@
   <dimension ref="A1:AD67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="12.75"/>
@@ -1748,16 +1487,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="2" t="s">
         <v>41</v>
       </c>
@@ -1789,15 +1528,15 @@
       <c r="H2" s="3">
         <v>2</v>
       </c>
-      <c r="I2" s="48">
-        <v>3</v>
-      </c>
-      <c r="J2" s="49">
+      <c r="I2" s="41">
+        <v>1</v>
+      </c>
+      <c r="J2" s="42">
         <v>1</v>
       </c>
       <c r="K2" s="3">
         <f>ROUNDUP(H2/(I2*J2),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="6"/>
     </row>
@@ -1818,15 +1557,15 @@
       <c r="H3" s="3">
         <v>8</v>
       </c>
-      <c r="I3" s="48">
-        <v>2</v>
-      </c>
-      <c r="J3" s="49">
+      <c r="I3" s="41">
+        <v>1</v>
+      </c>
+      <c r="J3" s="42">
         <v>1</v>
       </c>
       <c r="K3" s="3">
         <f t="shared" ref="K3:K13" si="0">ROUNDUP(H3/(I3*J3),0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L3" s="6"/>
     </row>
@@ -1849,10 +1588,10 @@
       <c r="H4" s="3">
         <v>8</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="41">
         <v>1</v>
       </c>
-      <c r="J4" s="49">
+      <c r="J4" s="42">
         <v>1</v>
       </c>
       <c r="K4" s="3">
@@ -1878,10 +1617,10 @@
       <c r="H5" s="3">
         <v>6</v>
       </c>
-      <c r="I5" s="48">
+      <c r="I5" s="41">
         <v>1</v>
       </c>
-      <c r="J5" s="49">
+      <c r="J5" s="42">
         <v>1</v>
       </c>
       <c r="K5" s="3">
@@ -1907,10 +1646,10 @@
       <c r="H6" s="3">
         <v>8</v>
       </c>
-      <c r="I6" s="48">
+      <c r="I6" s="41">
         <v>1</v>
       </c>
-      <c r="J6" s="49">
+      <c r="J6" s="42">
         <v>1</v>
       </c>
       <c r="K6" s="3">
@@ -1936,10 +1675,10 @@
       <c r="H7" s="3">
         <v>8</v>
       </c>
-      <c r="I7" s="48">
+      <c r="I7" s="41">
         <v>1</v>
       </c>
-      <c r="J7" s="49">
+      <c r="J7" s="42">
         <v>1</v>
       </c>
       <c r="K7" s="3">
@@ -1969,10 +1708,10 @@
       <c r="H8" s="3">
         <v>5</v>
       </c>
-      <c r="I8" s="48">
+      <c r="I8" s="41">
         <v>1</v>
       </c>
-      <c r="J8" s="49">
+      <c r="J8" s="42">
         <v>1</v>
       </c>
       <c r="K8" s="3">
@@ -1998,10 +1737,10 @@
       <c r="H9" s="3">
         <v>6</v>
       </c>
-      <c r="I9" s="48">
+      <c r="I9" s="41">
         <v>1</v>
       </c>
-      <c r="J9" s="49">
+      <c r="J9" s="42">
         <v>1</v>
       </c>
       <c r="K9" s="3">
@@ -2027,10 +1766,10 @@
       <c r="H10" s="3">
         <v>5</v>
       </c>
-      <c r="I10" s="48">
+      <c r="I10" s="41">
         <v>1</v>
       </c>
-      <c r="J10" s="49">
+      <c r="J10" s="42">
         <v>1</v>
       </c>
       <c r="K10" s="3">
@@ -2056,10 +1795,10 @@
       <c r="H11" s="3">
         <v>8</v>
       </c>
-      <c r="I11" s="48">
+      <c r="I11" s="41">
         <v>1</v>
       </c>
-      <c r="J11" s="49">
+      <c r="J11" s="42">
         <v>1</v>
       </c>
       <c r="K11" s="3">
@@ -2087,10 +1826,10 @@
       <c r="H12" s="3">
         <v>2</v>
       </c>
-      <c r="I12" s="48">
+      <c r="I12" s="41">
         <v>1</v>
       </c>
-      <c r="J12" s="49">
+      <c r="J12" s="42">
         <v>1</v>
       </c>
       <c r="K12" s="3">
@@ -2116,10 +1855,10 @@
       <c r="H13" s="3">
         <v>4</v>
       </c>
-      <c r="I13" s="48">
+      <c r="I13" s="41">
         <v>1</v>
       </c>
-      <c r="J13" s="49">
+      <c r="J13" s="42">
         <v>1</v>
       </c>
       <c r="K13" s="3">
@@ -2135,100 +1874,100 @@
       <c r="B15" s="16"/>
       <c r="C15" s="17">
         <f>A15+A17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F15" s="15">
         <f>C15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="17">
         <f>F15+F17</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K15" s="15">
         <f>H15</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15" s="17">
         <f>K15+K17</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="P15" s="15">
         <f>M15</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="Q15" s="16"/>
       <c r="R15" s="17">
         <f>P15+P17</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="U15" s="15">
         <f>R15</f>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="V15" s="16"/>
       <c r="W15" s="17">
         <f>U15+U17</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Z15" s="15">
         <f>MAX(W15,W20)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AA15" s="16"/>
       <c r="AB15" s="17">
         <f>Z15+Z17</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="13.5" thickBot="1">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="23"/>
       <c r="E16" s="24"/>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
       <c r="I16" s="23"/>
       <c r="J16" s="24"/>
-      <c r="K16" s="43" t="s">
+      <c r="K16" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="49"/>
       <c r="N16" s="23"/>
       <c r="O16" s="24"/>
-      <c r="P16" s="42" t="s">
+      <c r="P16" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="44"/>
       <c r="S16" s="23"/>
       <c r="T16" s="24"/>
-      <c r="U16" s="42" t="s">
+      <c r="U16" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="V16" s="42"/>
-      <c r="W16" s="42"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
       <c r="X16" s="23"/>
       <c r="Y16" s="24"/>
-      <c r="Z16" s="42" t="s">
+      <c r="Z16" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AA16" s="42"/>
-      <c r="AB16" s="42"/>
+      <c r="AA16" s="44"/>
+      <c r="AB16" s="44"/>
     </row>
     <row r="17" spans="1:30" ht="13.5" thickBot="1">
       <c r="A17" s="18">
         <f>VLOOKUP(A16,$A$2:$K$13,11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" s="19">
         <f>C18-C15</f>
@@ -2238,11 +1977,11 @@
       <c r="D17" s="25"/>
       <c r="F17" s="18">
         <f>VLOOKUP(F16,$A$2:$K$13,11)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G17" s="19">
         <f>H18-H15</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H17" s="20"/>
       <c r="K17" s="18">
@@ -2251,7 +1990,7 @@
       </c>
       <c r="L17" s="19">
         <f>M18-M15</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M17" s="20"/>
       <c r="P17" s="18">
@@ -2260,7 +1999,7 @@
       </c>
       <c r="Q17" s="19">
         <f>R18-R15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="20"/>
       <c r="U17" s="18">
@@ -2269,7 +2008,7 @@
       </c>
       <c r="V17" s="19">
         <f>W18-W15</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W17" s="20"/>
       <c r="Y17" s="30"/>
@@ -2294,12 +2033,12 @@
       <c r="B18" s="16"/>
       <c r="C18" s="22">
         <f>MIN(F18,F23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="26"/>
       <c r="F18" s="21">
         <f>H18-F17</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="22">
@@ -2316,31 +2055,32 @@
         <v>16</v>
       </c>
       <c r="P18" s="21">
+        <f>R18-P17</f>
         <v>16</v>
       </c>
       <c r="Q18" s="16"/>
       <c r="R18" s="22">
         <f>U18</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="U18" s="21">
         <f>W18-U17</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="V18" s="16"/>
       <c r="W18" s="22">
         <f>Z18</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="X18" s="27"/>
       <c r="Z18" s="21">
         <f>AB18-Z17</f>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AA18" s="16"/>
       <c r="AB18" s="22">
         <f>AB15</f>
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:30">
@@ -2351,71 +2091,71 @@
       <c r="D20" s="27"/>
       <c r="F20" s="15">
         <f>C15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="17">
         <f>F20+F22</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K20" s="15">
         <f>H20</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L20" s="16"/>
       <c r="M20" s="17">
         <f>K20+K22</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P20" s="15">
         <f>M20</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q20" s="16"/>
       <c r="R20" s="17">
         <f>P20+P22</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U20" s="15">
         <f>MAX(R20,R25)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V20" s="16"/>
       <c r="W20" s="17">
         <f>U20+U22</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="X20" s="27"/>
     </row>
     <row r="21" spans="1:30" ht="13.5" thickBot="1">
       <c r="D21" s="27"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="23"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="42" t="s">
+      <c r="K21" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
       <c r="N21" s="23"/>
       <c r="O21" s="24"/>
-      <c r="P21" s="42" t="s">
+      <c r="P21" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="44"/>
       <c r="S21" s="23"/>
       <c r="T21" s="24"/>
-      <c r="U21" s="42" t="s">
+      <c r="U21" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="V21" s="42"/>
-      <c r="W21" s="42"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
       <c r="X21" s="29"/>
     </row>
     <row r="22" spans="1:30" ht="13.5" thickBot="1">
@@ -2425,7 +2165,7 @@
       </c>
       <c r="G22" s="19">
         <f>H23-H20</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H22" s="20"/>
       <c r="I22" s="25"/>
@@ -2435,7 +2175,7 @@
       </c>
       <c r="L22" s="19">
         <f>M23-M20</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M22" s="20"/>
       <c r="P22" s="18">
@@ -2444,7 +2184,7 @@
       </c>
       <c r="Q22" s="19">
         <f>R23-R20</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R22" s="20"/>
       <c r="T22" s="24"/>
@@ -2454,48 +2194,48 @@
       </c>
       <c r="V22" s="19">
         <f>W23-W20</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W22" s="20"/>
     </row>
     <row r="23" spans="1:30">
       <c r="F23" s="21">
         <f>H23-F22</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="22">
         <f>MIN(K23,K28)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="I23" s="26"/>
       <c r="K23" s="21">
         <f>M23-K22</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L23" s="16"/>
       <c r="M23" s="22">
         <f>P23</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="P23" s="21">
         <f>R23-P22</f>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="Q23" s="16"/>
       <c r="R23" s="22">
         <f>U23</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="S23" s="27"/>
       <c r="U23" s="21">
         <f>W23-U22</f>
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="V23" s="16"/>
       <c r="W23" s="22">
         <f>Z18</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:30">
@@ -2506,39 +2246,39 @@
       <c r="I25" s="27"/>
       <c r="K25" s="15">
         <f>H20</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L25" s="16"/>
       <c r="M25" s="17">
         <f>K25+K27</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P25" s="15">
         <f>M25</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Q25" s="16"/>
       <c r="R25" s="17">
         <f>P25+P27</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="1:30" ht="13.5" thickBot="1">
       <c r="I26" s="27"/>
       <c r="J26" s="28"/>
-      <c r="K26" s="42" t="s">
+      <c r="K26" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="L26" s="42"/>
-      <c r="M26" s="42"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="44"/>
       <c r="N26" s="23"/>
       <c r="O26" s="24"/>
-      <c r="P26" s="42" t="s">
+      <c r="P26" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="Q26" s="42"/>
-      <c r="R26" s="42"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
       <c r="S26" s="29"/>
     </row>
     <row r="27" spans="1:30">
@@ -2547,6 +2287,7 @@
         <v>8</v>
       </c>
       <c r="L27" s="19">
+        <f>M28-M25</f>
         <v>4</v>
       </c>
       <c r="M27" s="20"/>
@@ -2556,28 +2297,28 @@
       </c>
       <c r="Q27" s="19">
         <f>R28-R25</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R27" s="20"/>
     </row>
     <row r="28" spans="1:30">
       <c r="K28" s="21">
         <f>M28-K27</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L28" s="16"/>
       <c r="M28" s="22">
         <f>P28</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="P28" s="21">
         <f>R28-P27</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="Q28" s="16"/>
       <c r="R28" s="22">
         <f>U23</f>
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="56.25">
@@ -2599,35 +2340,35 @@
       <c r="D36" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="46" t="s">
+      <c r="H36" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="43"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="43"/>
+      <c r="O36" s="43"/>
+      <c r="P36" s="43"/>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="H37" s="46" t="s">
+      <c r="A37" s="44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="44"/>
+      <c r="C37" s="44"/>
+      <c r="H37" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="43"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="43"/>
+      <c r="P37" s="43"/>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" s="18" t="s">
@@ -2642,17 +2383,17 @@
       <c r="D38" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="46" t="s">
+      <c r="H38" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="I38" s="46"/>
-      <c r="J38" s="46"/>
-      <c r="K38" s="46"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46"/>
-      <c r="O38" s="46"/>
-      <c r="P38" s="46"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="43"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="21" t="s">
@@ -2665,17 +2406,17 @@
       <c r="D39" t="s">
         <v>34</v>
       </c>
-      <c r="H39" s="46" t="s">
+      <c r="H39" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
-      <c r="K39" s="46"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="46"/>
-      <c r="N39" s="46"/>
-      <c r="O39" s="46"/>
-      <c r="P39" s="46"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
+      <c r="K39" s="43"/>
+      <c r="L39" s="43"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="43"/>
+      <c r="O39" s="43"/>
+      <c r="P39" s="43"/>
     </row>
     <row r="41" spans="1:16" ht="13.5">
       <c r="J41" s="9"/>
@@ -2759,11 +2500,11 @@
     </row>
     <row r="56" spans="1:11" ht="13.5">
       <c r="A56" s="8"/>
-      <c r="B56" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
+      <c r="B56" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="45"/>
+      <c r="D56" s="45"/>
       <c r="E56" s="10"/>
       <c r="F56" s="11" t="s">
         <v>18</v>
@@ -2933,6 +2674,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="Z16:AB16"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="U21:W21"/>
     <mergeCell ref="H36:P36"/>
     <mergeCell ref="H37:P37"/>
     <mergeCell ref="K26:M26"/>
@@ -2941,75 +2694,63 @@
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="H38:P38"/>
     <mergeCell ref="H39:P39"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="Z16:AB16"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="U21:W21"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="K16:M16"/>
   </mergeCells>
   <conditionalFormatting sqref="B17">
-    <cfRule type="cellIs" dxfId="72" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="cellIs" dxfId="71" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G17">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q17 Q27">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q22">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V17">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V22">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA17">
+    <cfRule type="cellIs" dxfId="32" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L27">
-    <cfRule type="cellIs" dxfId="66" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G17">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q17 Q27">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V17">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -3040,16 +2781,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3260,39 +3001,39 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="13.5" thickBot="1">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="23"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="23"/>
       <c r="J13" s="24"/>
-      <c r="K13" s="42" t="s">
+      <c r="K13" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
+      <c r="L13" s="44"/>
+      <c r="M13" s="44"/>
       <c r="N13" s="23"/>
       <c r="O13" s="24"/>
-      <c r="P13" s="42" t="s">
+      <c r="P13" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
       <c r="S13" s="23"/>
       <c r="T13" s="24"/>
-      <c r="U13" s="42" t="s">
+      <c r="U13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
     </row>
     <row r="14" spans="1:23" ht="13.5" thickBot="1">
       <c r="A14" s="18">
@@ -3424,25 +3165,25 @@
     <row r="19" spans="4:19" ht="13.5" thickBot="1">
       <c r="D19" s="27"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
       <c r="I19" s="23"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="42" t="s">
+      <c r="K19" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44"/>
       <c r="N19" s="23"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="42" t="s">
+      <c r="P19" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="44"/>
       <c r="S19" s="29"/>
     </row>
     <row r="20" spans="4:19" ht="13.5" thickBot="1">
@@ -3526,11 +3267,11 @@
     <row r="25" spans="4:19" ht="13.5" thickBot="1">
       <c r="I25" s="27"/>
       <c r="J25" s="28"/>
-      <c r="K25" s="42" t="s">
+      <c r="K25" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
       <c r="N25" s="29"/>
     </row>
     <row r="26" spans="4:19">
@@ -3556,65 +3297,65 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="K13:M13"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="U13:W13"/>
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="K19:M19"/>
     <mergeCell ref="P19:R19"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="K13:M13"/>
   </mergeCells>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="59" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="58" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8">
-    <cfRule type="cellIs" dxfId="56" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="54" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="53" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="52" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="50" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3644,16 +3385,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3809,16 +3550,16 @@
       <c r="H9" s="3">
         <v>15</v>
       </c>
-      <c r="P9" s="46" t="s">
+      <c r="P9" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="46"/>
-      <c r="R9" s="46"/>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
-      <c r="U9" s="46"/>
-      <c r="V9" s="46"/>
-      <c r="W9" s="46"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
     </row>
     <row r="10" spans="1:28">
       <c r="A10" s="3" t="s">
@@ -3882,18 +3623,18 @@
       </c>
     </row>
     <row r="13" spans="1:28" ht="13.5" thickBot="1">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="23"/>
       <c r="E13" s="24"/>
-      <c r="F13" s="42" t="s">
+      <c r="F13" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
       <c r="I13" s="23"/>
       <c r="J13" s="24"/>
       <c r="K13" s="23"/>
@@ -3901,21 +3642,21 @@
       <c r="M13" s="24"/>
       <c r="N13" s="23"/>
       <c r="O13" s="24"/>
-      <c r="P13" s="42" t="s">
+      <c r="P13" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
+      <c r="Q13" s="44"/>
+      <c r="R13" s="44"/>
       <c r="S13" s="23"/>
       <c r="T13" s="24"/>
-      <c r="U13" s="42" t="s">
+      <c r="U13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="V13" s="42"/>
-      <c r="W13" s="42"/>
-      <c r="Z13" s="42"/>
-      <c r="AA13" s="42"/>
-      <c r="AB13" s="42"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+      <c r="Z13" s="44"/>
+      <c r="AA13" s="44"/>
+      <c r="AB13" s="44"/>
     </row>
     <row r="14" spans="1:28" ht="13.5" thickBot="1">
       <c r="A14" s="18">
@@ -4069,25 +3810,25 @@
       <c r="C19" s="27"/>
       <c r="D19" s="27"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
       <c r="I19" s="23"/>
       <c r="J19" s="24"/>
-      <c r="K19" s="42" t="s">
+      <c r="K19" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L19" s="42"/>
-      <c r="M19" s="42"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="44"/>
       <c r="N19" s="23"/>
       <c r="O19" s="24"/>
-      <c r="P19" s="42" t="s">
+      <c r="P19" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="Q19" s="42"/>
-      <c r="R19" s="42"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="44"/>
       <c r="S19" s="29"/>
     </row>
     <row r="20" spans="3:19" ht="13.5" thickBot="1">
@@ -4196,18 +3937,18 @@
       <c r="C25" s="27"/>
       <c r="D25" s="36"/>
       <c r="E25" s="24"/>
-      <c r="F25" s="42" t="s">
+      <c r="F25" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="42"/>
-      <c r="H25" s="43"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="47"/>
       <c r="I25" s="37"/>
       <c r="J25" s="37"/>
-      <c r="K25" s="45" t="s">
+      <c r="K25" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="L25" s="44"/>
+      <c r="M25" s="44"/>
       <c r="N25" s="29"/>
     </row>
     <row r="26" spans="3:19">
@@ -4258,6 +3999,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="P9:W9"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
     <mergeCell ref="Z13:AB13"/>
     <mergeCell ref="F25:H25"/>
     <mergeCell ref="U13:W13"/>
@@ -4266,59 +4012,54 @@
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P9:W9"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
   </mergeCells>
   <conditionalFormatting sqref="B14">
-    <cfRule type="cellIs" dxfId="49" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="40" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20">
-    <cfRule type="cellIs" dxfId="39" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G26">
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="37" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26">
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q14">
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q20">
-    <cfRule type="cellIs" dxfId="34" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V14">
-    <cfRule type="cellIs" dxfId="33" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4348,16 +4089,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4608,18 +4349,18 @@
       </c>
     </row>
     <row r="15" spans="1:24" ht="13.5" thickBot="1">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="23"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
       <c r="I15" s="23"/>
       <c r="J15" s="24"/>
       <c r="K15" s="23"/>
@@ -4627,18 +4368,18 @@
       <c r="M15" s="24"/>
       <c r="N15" s="23"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="42" t="s">
+      <c r="P15" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
       <c r="S15" s="23"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="42" t="s">
+      <c r="U15" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="V15" s="42"/>
-      <c r="W15" s="42"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
       <c r="X15" s="23"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" thickBot="1">
@@ -4748,11 +4489,11 @@
     <row r="18" spans="1:28">
       <c r="C18" s="35"/>
       <c r="D18" s="27"/>
-      <c r="Z18" s="43" t="s">
+      <c r="Z18" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="AA18" s="44"/>
-      <c r="AB18" s="45"/>
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
     </row>
     <row r="19" spans="1:28" ht="13.5" thickBot="1">
       <c r="C19" s="27"/>
@@ -4824,32 +4565,32 @@
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="42" t="s">
+      <c r="F21" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
+      <c r="G21" s="44"/>
+      <c r="H21" s="44"/>
       <c r="I21" s="23"/>
       <c r="J21" s="24"/>
-      <c r="K21" s="42" t="s">
+      <c r="K21" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
+      <c r="L21" s="44"/>
+      <c r="M21" s="44"/>
       <c r="N21" s="23"/>
       <c r="O21" s="24"/>
-      <c r="P21" s="42" t="s">
+      <c r="P21" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="43"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="47"/>
       <c r="S21" s="37"/>
       <c r="T21" s="37"/>
-      <c r="U21" s="45" t="s">
+      <c r="U21" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="V21" s="42"/>
-      <c r="W21" s="42"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44"/>
       <c r="X21" s="29"/>
     </row>
     <row r="22" spans="1:28" ht="13.5" thickBot="1">
@@ -4979,18 +4720,18 @@
       <c r="C27" s="27"/>
       <c r="D27" s="36"/>
       <c r="E27" s="24"/>
-      <c r="F27" s="42" t="s">
+      <c r="F27" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="42"/>
-      <c r="H27" s="43"/>
+      <c r="G27" s="44"/>
+      <c r="H27" s="47"/>
       <c r="I27" s="37"/>
       <c r="J27" s="37"/>
-      <c r="K27" s="45" t="s">
+      <c r="K27" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="42"/>
-      <c r="M27" s="42"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="44"/>
       <c r="N27" s="29"/>
     </row>
     <row r="28" spans="1:28">
@@ -5041,12 +4782,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="P15:R15"/>
     <mergeCell ref="Z18:AB18"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="K21:M21"/>
@@ -5054,59 +4789,65 @@
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="K27:M27"/>
     <mergeCell ref="U21:W21"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="P15:R15"/>
   </mergeCells>
   <conditionalFormatting sqref="B16">
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G16">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G22">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G28">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L22">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L28">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q22">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V22">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA19">
-    <cfRule type="cellIs" dxfId="16" priority="7" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="V22">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q22">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L22">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G22">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>